<commit_message>
added incident report download functionality to frontend
</commit_message>
<xml_diff>
--- a/public/assets/incidentsReport.xlsx
+++ b/public/assets/incidentsReport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S530468\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S530468\Desktop\Backend-Working Version\New\DisasterResponseAndReportingSystem-Backend\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,17 +24,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Testing</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Incident Name</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Earthquake</t>
+  </si>
+  <si>
+    <t>Maryville</t>
+  </si>
+  <si>
+    <t>Goldfinger was two hundred miles away, in the city of Kashiwa, at an international meeting on seismology.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -62,8 +91,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -344,20 +383,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43356</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>